<commit_message>
Got 3-methyl-heptane data written in correct ChemKED format. Data has been verified
</commit_message>
<xml_diff>
--- a/3-methyl-heptane/wang_shock_tube.xlsx
+++ b/3-methyl-heptane/wang_shock_tube.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Code/OOHabstraction/comparisonTST/reference_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Code/OOHabstraction/comparisonTST/reference_files/wang_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B04B6A3-8E18-AB4B-9884-14251FC2C7D5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RPI shock tube" sheetId="1" r:id="rId1"/>
     <sheet name="NUIG shock tube" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -210,6 +211,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -477,11 +481,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1668,11 +1672,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1681,11 +1685,11 @@
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -1695,11 +1699,11 @@
       <c r="A2">
         <v>0.5</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="7">
+        <v>6.66</v>
+      </c>
+      <c r="C2" s="9">
         <v>1086</v>
-      </c>
-      <c r="C2" s="7">
-        <v>6.66</v>
       </c>
       <c r="D2" s="8">
         <v>984</v>
@@ -1709,11 +1713,11 @@
       <c r="A3">
         <v>0.5</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
+        <v>7.11</v>
+      </c>
+      <c r="C3" s="9">
         <v>1089</v>
-      </c>
-      <c r="C3" s="7">
-        <v>7.11</v>
       </c>
       <c r="D3" s="8">
         <v>1072</v>
@@ -1723,11 +1727,11 @@
       <c r="A4">
         <v>0.5</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
+        <v>7</v>
+      </c>
+      <c r="C4" s="9">
         <v>1169</v>
-      </c>
-      <c r="C4" s="7">
-        <v>7</v>
       </c>
       <c r="D4" s="8">
         <v>560</v>
@@ -1737,11 +1741,11 @@
       <c r="A5">
         <v>0.5</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
+        <v>6.56</v>
+      </c>
+      <c r="C5" s="9">
         <v>1253</v>
-      </c>
-      <c r="C5" s="7">
-        <v>6.56</v>
       </c>
       <c r="D5" s="8">
         <v>151</v>
@@ -1751,11 +1755,11 @@
       <c r="A6">
         <v>0.5</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
+        <v>6.04</v>
+      </c>
+      <c r="C6" s="9">
         <v>1261</v>
-      </c>
-      <c r="C6" s="7">
-        <v>6.04</v>
       </c>
       <c r="D6" s="8">
         <v>116</v>
@@ -1765,11 +1769,11 @@
       <c r="A7">
         <v>0.5</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
+        <v>10.79</v>
+      </c>
+      <c r="C7" s="9">
         <v>1058</v>
-      </c>
-      <c r="C7" s="7">
-        <v>10.79</v>
       </c>
       <c r="D7" s="8">
         <v>1625</v>
@@ -1779,11 +1783,11 @@
       <c r="A8">
         <v>0.5</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="C8" s="9">
         <v>1097</v>
-      </c>
-      <c r="C8" s="7">
-        <v>9.4700000000000006</v>
       </c>
       <c r="D8" s="8">
         <v>700</v>
@@ -1793,11 +1797,11 @@
       <c r="A9">
         <v>0.5</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="C9" s="9">
         <v>1211</v>
-      </c>
-      <c r="C9" s="7">
-        <v>9.3800000000000008</v>
       </c>
       <c r="D9" s="8">
         <v>192</v>
@@ -1807,11 +1811,11 @@
       <c r="A10">
         <v>0.5</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
+        <v>8.24</v>
+      </c>
+      <c r="C10" s="9">
         <v>1311</v>
-      </c>
-      <c r="C10" s="7">
-        <v>8.24</v>
       </c>
       <c r="D10" s="8">
         <v>54</v>
@@ -1822,10 +1826,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="7">
+        <v>7.34</v>
+      </c>
+      <c r="C11" s="7">
         <v>1091</v>
-      </c>
-      <c r="C11" s="7">
-        <v>7.34</v>
       </c>
       <c r="D11" s="8">
         <v>1176</v>
@@ -1836,10 +1840,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="7">
+        <v>7.02</v>
+      </c>
+      <c r="C12" s="7">
         <v>1094</v>
-      </c>
-      <c r="C12" s="7">
-        <v>7.02</v>
       </c>
       <c r="D12" s="8">
         <v>880</v>
@@ -1850,10 +1854,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="7">
+        <v>7.06</v>
+      </c>
+      <c r="C13" s="7">
         <v>1123</v>
-      </c>
-      <c r="C13" s="7">
-        <v>7.06</v>
       </c>
       <c r="D13" s="8">
         <v>562</v>
@@ -1864,10 +1868,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="7">
+        <v>6.53</v>
+      </c>
+      <c r="C14" s="7">
         <v>1246</v>
-      </c>
-      <c r="C14" s="7">
-        <v>6.53</v>
       </c>
       <c r="D14" s="8">
         <v>184</v>
@@ -1878,10 +1882,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="7">
+        <v>11.16</v>
+      </c>
+      <c r="C15" s="7">
         <v>955</v>
-      </c>
-      <c r="C15" s="7">
-        <v>11.16</v>
       </c>
       <c r="D15" s="8">
         <v>2550</v>
@@ -1892,10 +1896,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="5">
+        <v>11.21</v>
+      </c>
+      <c r="C16" s="5">
         <v>1039</v>
-      </c>
-      <c r="C16" s="5">
-        <v>11.21</v>
       </c>
       <c r="D16" s="6">
         <v>1029</v>
@@ -1906,10 +1910,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="7">
+        <v>11.09</v>
+      </c>
+      <c r="C17" s="7">
         <v>1040</v>
-      </c>
-      <c r="C17" s="7">
-        <v>11.09</v>
       </c>
       <c r="D17" s="8">
         <v>1115</v>
@@ -1920,10 +1924,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="5">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="C18" s="5">
         <v>1118</v>
-      </c>
-      <c r="C18" s="5">
-        <v>10.220000000000001</v>
       </c>
       <c r="D18" s="6">
         <v>391</v>
@@ -1934,10 +1938,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="7">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="C19" s="7">
         <v>1125</v>
-      </c>
-      <c r="C19" s="7">
-        <v>9.5399999999999991</v>
       </c>
       <c r="D19" s="8">
         <v>370</v>
@@ -1948,10 +1952,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="5">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="C20" s="5">
         <v>1204</v>
-      </c>
-      <c r="C20" s="5">
-        <v>10.119999999999999</v>
       </c>
       <c r="D20" s="6">
         <v>193</v>
@@ -1962,10 +1966,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="7">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="C21" s="7">
         <v>1294</v>
-      </c>
-      <c r="C21" s="7">
-        <v>8.8699999999999992</v>
       </c>
       <c r="D21" s="8">
         <v>68</v>
@@ -1976,10 +1980,10 @@
         <v>1</v>
       </c>
       <c r="B22" s="2">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="C22" s="2">
         <v>1356</v>
-      </c>
-      <c r="C22" s="2">
-        <v>8.2799999999999994</v>
       </c>
       <c r="D22" s="3">
         <v>40</v>
@@ -1990,10 +1994,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="7">
+        <v>7.28</v>
+      </c>
+      <c r="C23" s="7">
         <v>1077</v>
-      </c>
-      <c r="C23" s="7">
-        <v>7.28</v>
       </c>
       <c r="D23" s="8">
         <v>1311</v>
@@ -2004,10 +2008,10 @@
         <v>2</v>
       </c>
       <c r="B24" s="7">
+        <v>6.84</v>
+      </c>
+      <c r="C24" s="7">
         <v>1135</v>
-      </c>
-      <c r="C24" s="7">
-        <v>6.84</v>
       </c>
       <c r="D24" s="8">
         <v>735</v>
@@ -2018,10 +2022,10 @@
         <v>2</v>
       </c>
       <c r="B25" s="7">
+        <v>5.51</v>
+      </c>
+      <c r="C25" s="7">
         <v>1148</v>
-      </c>
-      <c r="C25" s="7">
-        <v>5.51</v>
       </c>
       <c r="D25" s="8">
         <v>483</v>
@@ -2031,11 +2035,11 @@
       <c r="A26">
         <v>2</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="7">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="C26" s="5">
         <v>1225</v>
-      </c>
-      <c r="C26" s="7">
-        <v>4.5599999999999996</v>
       </c>
       <c r="D26" s="8">
         <v>222</v>
@@ -2046,10 +2050,10 @@
         <v>2</v>
       </c>
       <c r="B27" s="7">
+        <v>10.19</v>
+      </c>
+      <c r="C27" s="7">
         <v>1001</v>
-      </c>
-      <c r="C27" s="7">
-        <v>10.19</v>
       </c>
       <c r="D27" s="8">
         <v>1146</v>
@@ -2060,10 +2064,10 @@
         <v>2</v>
       </c>
       <c r="B28" s="7">
+        <v>10.029999999999999</v>
+      </c>
+      <c r="C28" s="7">
         <v>1054</v>
-      </c>
-      <c r="C28" s="7">
-        <v>10.029999999999999</v>
       </c>
       <c r="D28" s="8">
         <v>823</v>
@@ -2074,10 +2078,10 @@
         <v>2</v>
       </c>
       <c r="B29" s="7">
+        <v>9.32</v>
+      </c>
+      <c r="C29" s="7">
         <v>1089</v>
-      </c>
-      <c r="C29" s="7">
-        <v>9.32</v>
       </c>
       <c r="D29" s="8">
         <v>497</v>
@@ -2088,10 +2092,10 @@
         <v>2</v>
       </c>
       <c r="B30" s="7">
+        <v>9.24</v>
+      </c>
+      <c r="C30" s="7">
         <v>1237</v>
-      </c>
-      <c r="C30" s="7">
-        <v>9.24</v>
       </c>
       <c r="D30" s="8">
         <v>152</v>
@@ -2101,11 +2105,11 @@
       <c r="A31">
         <v>2</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="7">
+        <v>7.57</v>
+      </c>
+      <c r="C31" s="5">
         <v>1351</v>
-      </c>
-      <c r="C31" s="7">
-        <v>7.57</v>
       </c>
       <c r="D31" s="8">
         <v>47</v>

</xml_diff>

<commit_message>
Added RCM data, verified by ChemKED
</commit_message>
<xml_diff>
--- a/3-methyl-heptane/wang_shock_tube.xlsx
+++ b/3-methyl-heptane/wang_shock_tube.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Code/OOHabstraction/comparisonTST/reference_files/wang_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Code/ChemKED-database/3-methyl-heptane/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B04B6A3-8E18-AB4B-9884-14251FC2C7D5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DA8842-FBA2-1C47-8393-DD691D79FD84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-8920" windowWidth="19160" windowHeight="21600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RPI shock tube" sheetId="1" r:id="rId1"/>
-    <sheet name="NUIG shock tube" sheetId="2" r:id="rId2"/>
+    <sheet name="NUID RCM" sheetId="3" r:id="rId2"/>
+    <sheet name="NUIG shock tube" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>P [atm]</t>
   </si>
@@ -42,12 +43,168 @@
   <si>
     <t xml:space="preserve">φ </t>
   </si>
+  <si>
+    <t>Diluent</t>
+  </si>
+  <si>
+    <r>
+      <t>CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [atm]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [K]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [atm]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [K]</t>
+    </r>
+  </si>
+  <si>
+    <t>τ [ms]</t>
+  </si>
+  <si>
+    <t>first stage heat loss [ms]</t>
+  </si>
+  <si>
+    <t>0/100</t>
+  </si>
+  <si>
+    <t>50/50</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,6 +240,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -92,7 +264,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -162,13 +334,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -199,6 +402,39 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -484,7 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -1672,6 +1908,416 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE7B2C5-401D-8546-BBFE-71406709016E}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.4214</v>
+      </c>
+      <c r="C3" s="11">
+        <v>373</v>
+      </c>
+      <c r="D3" s="11">
+        <v>9.73</v>
+      </c>
+      <c r="E3" s="11">
+        <v>825</v>
+      </c>
+      <c r="F3" s="11">
+        <v>39.6</v>
+      </c>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.4234</v>
+      </c>
+      <c r="C4" s="11">
+        <v>373</v>
+      </c>
+      <c r="D4" s="11">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="E4" s="11">
+        <v>822</v>
+      </c>
+      <c r="F4" s="11">
+        <v>40</v>
+      </c>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0.4244</v>
+      </c>
+      <c r="C5" s="11">
+        <v>383</v>
+      </c>
+      <c r="D5" s="11">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="E5" s="11">
+        <v>841</v>
+      </c>
+      <c r="F5" s="11">
+        <v>40.4</v>
+      </c>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0.4264</v>
+      </c>
+      <c r="C6" s="11">
+        <v>383</v>
+      </c>
+      <c r="D6" s="11">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="E6" s="11">
+        <v>840</v>
+      </c>
+      <c r="F6" s="11">
+        <v>42.2</v>
+      </c>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.4244</v>
+      </c>
+      <c r="C7" s="11">
+        <v>393</v>
+      </c>
+      <c r="D7" s="11">
+        <v>9.5</v>
+      </c>
+      <c r="E7" s="11">
+        <v>858</v>
+      </c>
+      <c r="F7" s="11">
+        <v>40</v>
+      </c>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0.4264</v>
+      </c>
+      <c r="C8" s="11">
+        <v>393</v>
+      </c>
+      <c r="D8" s="11">
+        <v>9.42</v>
+      </c>
+      <c r="E8" s="11">
+        <v>855</v>
+      </c>
+      <c r="F8" s="11">
+        <v>38.5</v>
+      </c>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0.43619999999999998</v>
+      </c>
+      <c r="C9" s="11">
+        <v>403</v>
+      </c>
+      <c r="D9" s="11">
+        <v>9.65</v>
+      </c>
+      <c r="E9" s="11">
+        <v>875</v>
+      </c>
+      <c r="F9" s="11">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="11">
+        <v>0.43619999999999998</v>
+      </c>
+      <c r="C10" s="11">
+        <v>403</v>
+      </c>
+      <c r="D10" s="11">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="E10" s="11">
+        <v>874</v>
+      </c>
+      <c r="F10" s="11">
+        <v>27.7</v>
+      </c>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="11">
+        <v>0.43519999999999998</v>
+      </c>
+      <c r="C11" s="11">
+        <v>413</v>
+      </c>
+      <c r="D11" s="11">
+        <v>9.68</v>
+      </c>
+      <c r="E11" s="11">
+        <v>895</v>
+      </c>
+      <c r="F11" s="11">
+        <v>22.4</v>
+      </c>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11">
+        <v>0.44119999999999998</v>
+      </c>
+      <c r="C12" s="11">
+        <v>413</v>
+      </c>
+      <c r="D12" s="11">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="E12" s="11">
+        <v>889</v>
+      </c>
+      <c r="F12" s="11">
+        <v>25.9</v>
+      </c>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="14"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11">
+        <v>0.49540000000000001</v>
+      </c>
+      <c r="C14" s="11">
+        <v>373</v>
+      </c>
+      <c r="D14" s="11">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="E14" s="11">
+        <v>714</v>
+      </c>
+      <c r="F14" s="11">
+        <v>23.1</v>
+      </c>
+      <c r="G14" s="15">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0.49349999999999999</v>
+      </c>
+      <c r="C15" s="11">
+        <v>373</v>
+      </c>
+      <c r="D15" s="11">
+        <v>9.92</v>
+      </c>
+      <c r="E15" s="11">
+        <v>714</v>
+      </c>
+      <c r="F15" s="11">
+        <v>23.7</v>
+      </c>
+      <c r="G15" s="15">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="11">
+        <v>0.49640000000000001</v>
+      </c>
+      <c r="C16" s="11">
+        <v>388</v>
+      </c>
+      <c r="D16" s="11">
+        <v>9.98</v>
+      </c>
+      <c r="E16" s="11">
+        <v>738</v>
+      </c>
+      <c r="F16" s="11">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="G16" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="11">
+        <v>0.49349999999999999</v>
+      </c>
+      <c r="C17" s="11">
+        <v>388</v>
+      </c>
+      <c r="D17" s="11">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="E17" s="11">
+        <v>737</v>
+      </c>
+      <c r="F17" s="11">
+        <v>19.7</v>
+      </c>
+      <c r="G17" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="11">
+        <v>0.49349999999999999</v>
+      </c>
+      <c r="C18" s="11">
+        <v>413</v>
+      </c>
+      <c r="D18" s="11">
+        <v>10.07</v>
+      </c>
+      <c r="E18" s="11">
+        <v>781</v>
+      </c>
+      <c r="F18" s="11">
+        <v>20.8</v>
+      </c>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="16">
+        <v>0.49440000000000001</v>
+      </c>
+      <c r="C19" s="16">
+        <v>413</v>
+      </c>
+      <c r="D19" s="16">
+        <v>10.18</v>
+      </c>
+      <c r="E19" s="16">
+        <v>782</v>
+      </c>
+      <c r="F19" s="16">
+        <v>21</v>
+      </c>
+      <c r="G19" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>

</xml_diff>